<commit_message>
Sprint Backlog 2 + Burndown Chart fix
Ändrade så jag har 5 dagar på mig och ändrade skattad och ideal tid
</commit_message>
<xml_diff>
--- a/Sprint Backlog 2.xlsx
+++ b/Sprint Backlog 2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Ändra skrivbordsbild</t>
+  </si>
+  <si>
+    <t>Dag 5</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -281,7 +284,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -290,6 +293,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -328,15 +334,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -354,11 +363,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="136954880"/>
-        <c:axId val="96948160"/>
+        <c:axId val="126862336"/>
+        <c:axId val="86790080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136954880"/>
+        <c:axId val="126862336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -367,7 +376,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96948160"/>
+        <c:crossAx val="86790080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -375,7 +384,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96948160"/>
+        <c:axId val="86790080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -401,7 +410,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136954880"/>
+        <c:crossAx val="126862336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -743,7 +752,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -787,7 +796,9 @@
       <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9"/>
+      <c r="J1" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -804,7 +815,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -813,6 +824,9 @@
         <v>0</v>
       </c>
       <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>0</v>
       </c>
     </row>
@@ -840,6 +854,9 @@
         <v>0</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>0</v>
       </c>
     </row>
@@ -856,7 +873,7 @@
         <v>8</v>
       </c>
       <c r="F6">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -865,6 +882,9 @@
         <v>0</v>
       </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>0</v>
       </c>
       <c r="M6" s="2"/>
@@ -874,15 +894,18 @@
         <v>9</v>
       </c>
       <c r="F7">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Burndown Chart 2 Update
</commit_message>
<xml_diff>
--- a/Sprint Backlog 2.xlsx
+++ b/Sprint Backlog 2.xlsx
@@ -287,7 +287,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -363,11 +363,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126862336"/>
-        <c:axId val="86790080"/>
+        <c:axId val="125420544"/>
+        <c:axId val="85413824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126862336"/>
+        <c:axId val="125420544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +376,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86790080"/>
+        <c:crossAx val="85413824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -384,7 +384,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86790080"/>
+        <c:axId val="85413824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,7 +410,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126862336"/>
+        <c:crossAx val="125420544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -752,7 +752,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -818,7 +818,7 @@
         <v>10</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -848,7 +848,7 @@
         <v>3</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -876,7 +876,7 @@
         <v>13</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H6">
         <v>0</v>

</xml_diff>

<commit_message>
Burndown Chart Update 2 igen
Tog litet uppehåll för jag var tvungen att fokusera på att jobba med
onlinetest men jobbade idag med projektet så jag uppdaterar nu
</commit_message>
<xml_diff>
--- a/Sprint Backlog 2.xlsx
+++ b/Sprint Backlog 2.xlsx
@@ -290,7 +290,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -363,11 +363,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="125420544"/>
-        <c:axId val="85413824"/>
+        <c:axId val="119915520"/>
+        <c:axId val="82005952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="125420544"/>
+        <c:axId val="119915520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +376,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85413824"/>
+        <c:crossAx val="82005952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -384,7 +384,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85413824"/>
+        <c:axId val="82005952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,7 +410,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125420544"/>
+        <c:crossAx val="119915520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -752,7 +752,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -821,7 +821,7 @@
         <v>5</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -879,7 +879,7 @@
         <v>8</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I6">
         <v>0</v>

</xml_diff>

<commit_message>
Fixat felaktiga ideal värden på Burndown Chart 2
Vet ej vad jag tänkte, men jag ändrade värderna till de som de ska vara
</commit_message>
<xml_diff>
--- a/Sprint Backlog 2.xlsx
+++ b/Sprint Backlog 2.xlsx
@@ -365,13 +365,13 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>9.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -391,11 +391,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="129614848"/>
-        <c:axId val="90001344"/>
+        <c:axId val="134267904"/>
+        <c:axId val="93605824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="129614848"/>
+        <c:axId val="134267904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,7 +404,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90001344"/>
+        <c:crossAx val="93605824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -412,7 +412,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90001344"/>
+        <c:axId val="93605824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -438,7 +438,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129614848"/>
+        <c:crossAx val="134267904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -780,7 +780,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -944,13 +944,13 @@
         <v>13</v>
       </c>
       <c r="G7">
-        <v>8</v>
+        <v>9.75</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>3.25</v>
       </c>
       <c r="J7">
         <v>0</v>

</xml_diff>

<commit_message>
Fix på Sprint Backlog 2
Glömt att ändra status på uppgifterna
</commit_message>
<xml_diff>
--- a/Sprint Backlog 2.xlsx
+++ b/Sprint Backlog 2.xlsx
@@ -49,9 +49,6 @@
     <t>Tider</t>
   </si>
   <si>
-    <t>Ej Färdig</t>
-  </si>
-  <si>
     <t>Som användare vill jag ha ett fotogalleri med tumnagelbilder</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>Funkar som förväntat</t>
+  </si>
+  <si>
+    <t>Klar</t>
   </si>
 </sst>
 </file>
@@ -391,11 +391,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="134267904"/>
-        <c:axId val="93605824"/>
+        <c:axId val="136299520"/>
+        <c:axId val="95637440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134267904"/>
+        <c:axId val="136299520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,7 +404,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93605824"/>
+        <c:crossAx val="95637440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -412,7 +412,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93605824"/>
+        <c:axId val="95637440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -438,7 +438,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134267904"/>
+        <c:crossAx val="136299520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -780,7 +780,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -826,13 +826,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -840,13 +840,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2">
@@ -865,10 +865,10 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
@@ -876,13 +876,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3">
@@ -901,10 +901,10 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Klar med SCRUM för projektet färdig
</commit_message>
<xml_diff>
--- a/Sprint Backlog 2.xlsx
+++ b/Sprint Backlog 2.xlsx
@@ -215,10 +215,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -391,11 +391,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="136299520"/>
-        <c:axId val="95637440"/>
+        <c:axId val="126731264"/>
+        <c:axId val="86069184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136299520"/>
+        <c:axId val="126731264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,7 +404,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95637440"/>
+        <c:crossAx val="86069184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -412,7 +412,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95637440"/>
+        <c:axId val="86069184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -438,7 +438,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136299520"/>
+        <c:crossAx val="126731264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -780,7 +780,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -825,13 +825,13 @@
       <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>